<commit_message>
rerun q1. And update analyser. histogram restored
</commit_message>
<xml_diff>
--- a/output_Q1/DF_Full_Result.xlsx
+++ b/output_Q1/DF_Full_Result.xlsx
@@ -76,31 +76,31 @@
     <t>softmax</t>
   </si>
   <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 15, 'epochs': 23, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 15, 'epochs': 20, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 20, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 20, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 20, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 23, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 15, 'epochs': 20, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
+    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 23, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
+  </si>
+  <si>
     <t>{'anOptimizer': 'adam', 'batch_size': 15, 'epochs': 23, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 15, 'epochs': 20, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 15, 'epochs': 20, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 15, 'epochs': 23, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 20, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 20, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 20, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 23, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
-  </si>
-  <si>
-    <t>{'anOptimizer': 'adam', 'batch_size': 20, 'epochs': 23, 'hidUnit': 256, 'outActivation': 'sigmoid'}</t>
   </si>
   <si>
     <t>{'anOptimizer': 'rmsprop', 'batch_size': 20, 'epochs': 20, 'hidUnit': 128, 'outActivation': 'sigmoid'}</t>
@@ -585,19 +585,19 @@
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="1">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B2">
-        <v>1.89487091700236</v>
+        <v>1.234651327133179</v>
       </c>
       <c r="C2">
-        <v>0.04917133899547547</v>
+        <v>0.01276819854875775</v>
       </c>
       <c r="D2">
-        <v>0.3223050435384114</v>
+        <v>0.1890469392140706</v>
       </c>
       <c r="E2">
-        <v>0.1437506495418769</v>
+        <v>0.005211298684879465</v>
       </c>
       <c r="F2" t="s">
         <v>16</v>
@@ -609,7 +609,7 @@
         <v>23</v>
       </c>
       <c r="I2">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="J2" t="s">
         <v>18</v>
@@ -641,16 +641,16 @@
         <v>31</v>
       </c>
       <c r="B3">
-        <v>1.630072911580404</v>
+        <v>1.320182085037231</v>
       </c>
       <c r="C3">
-        <v>0.1737224959153814</v>
+        <v>0.119534095731496</v>
       </c>
       <c r="D3">
-        <v>0.2399005889892578</v>
+        <v>0.1881728172302246</v>
       </c>
       <c r="E3">
-        <v>0.01189654589060991</v>
+        <v>0.001456219200621047</v>
       </c>
       <c r="F3" t="s">
         <v>16</v>
@@ -691,25 +691,25 @@
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="1">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>1.888932943344116</v>
+        <v>1.093486785888672</v>
       </c>
       <c r="C4">
-        <v>0.06233511502657465</v>
+        <v>0.01382945518987775</v>
       </c>
       <c r="D4">
-        <v>0.2352720101674398</v>
+        <v>0.1775549252827962</v>
       </c>
       <c r="E4">
-        <v>0.01274297381734479</v>
+        <v>0.002173349753314483</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G4">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H4">
         <v>20</v>
@@ -724,10 +724,10 @@
         <v>22</v>
       </c>
       <c r="L4">
+        <v>0.9632353186607361</v>
+      </c>
+      <c r="M4">
         <v>0.970588207244873</v>
-      </c>
-      <c r="M4">
-        <v>0.9632353186607361</v>
       </c>
       <c r="N4">
         <v>0.9485294222831726</v>
@@ -744,31 +744,31 @@
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="1">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B5">
-        <v>1.50573468208313</v>
+        <v>1.324541727701823</v>
       </c>
       <c r="C5">
-        <v>0.07384847079412747</v>
+        <v>0.06013406867044717</v>
       </c>
       <c r="D5">
-        <v>0.2351662317911784</v>
+        <v>0.2074383099873861</v>
       </c>
       <c r="E5">
-        <v>0.0104427927709632</v>
+        <v>0.02056102853352101</v>
       </c>
       <c r="F5" t="s">
         <v>16</v>
       </c>
       <c r="G5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H5">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I5">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="J5" t="s">
         <v>18</v>
@@ -777,19 +777,19 @@
         <v>23</v>
       </c>
       <c r="L5">
-        <v>0.9632353186607361</v>
+        <v>0.9852941036224365</v>
       </c>
       <c r="M5">
-        <v>0.970588207244873</v>
+        <v>0.9558823704719543</v>
       </c>
       <c r="N5">
-        <v>0.9485294222831726</v>
+        <v>0.9411764740943909</v>
       </c>
       <c r="O5">
         <v>0.9607843160629272</v>
       </c>
       <c r="P5">
-        <v>0.009170716395043688</v>
+        <v>0.01834144872006417</v>
       </c>
       <c r="Q5">
         <v>2</v>
@@ -797,22 +797,22 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="1">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="B6">
-        <v>1.326967795689901</v>
+        <v>1.293554862340291</v>
       </c>
       <c r="C6">
-        <v>0.09583365248827488</v>
+        <v>0.1613239823198422</v>
       </c>
       <c r="D6">
-        <v>0.2088305950164795</v>
+        <v>0.1985015074412028</v>
       </c>
       <c r="E6">
-        <v>0.00167230778574013</v>
+        <v>0.009949126504046411</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G6">
         <v>20</v>
@@ -821,7 +821,7 @@
         <v>20</v>
       </c>
       <c r="I6">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="J6" t="s">
         <v>18</v>
@@ -830,7 +830,7 @@
         <v>24</v>
       </c>
       <c r="L6">
-        <v>0.9632353186607361</v>
+        <v>0.9558823704719543</v>
       </c>
       <c r="M6">
         <v>0.970588207244873</v>
@@ -839,30 +839,30 @@
         <v>0.9485294222831726</v>
       </c>
       <c r="O6">
-        <v>0.9607843160629272</v>
+        <v>0.9583333333333334</v>
       </c>
       <c r="P6">
-        <v>0.009170716395043688</v>
+        <v>0.009170711085026055</v>
       </c>
       <c r="Q6">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="1">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B7">
-        <v>1.428937673568726</v>
+        <v>1.131050268809001</v>
       </c>
       <c r="C7">
-        <v>0.1490452562674241</v>
+        <v>0.006693242029809475</v>
       </c>
       <c r="D7">
-        <v>0.2594961325327556</v>
+        <v>0.1885590553283691</v>
       </c>
       <c r="E7">
-        <v>0.02980838061067517</v>
+        <v>0.01264984752100787</v>
       </c>
       <c r="F7" t="s">
         <v>16</v>
@@ -871,7 +871,7 @@
         <v>20</v>
       </c>
       <c r="H7">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="I7">
         <v>128</v>
@@ -883,45 +883,45 @@
         <v>25</v>
       </c>
       <c r="L7">
-        <v>0.9632353186607361</v>
+        <v>0.9779411554336548</v>
       </c>
       <c r="M7">
         <v>0.970588207244873</v>
       </c>
       <c r="N7">
-        <v>0.9485294222831726</v>
+        <v>0.9264705777168274</v>
       </c>
       <c r="O7">
-        <v>0.9607843160629272</v>
+        <v>0.9583333134651184</v>
       </c>
       <c r="P7">
-        <v>0.009170716395043688</v>
+        <v>0.02272945092152168</v>
       </c>
       <c r="Q7">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="1">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B8">
-        <v>1.565131425857544</v>
+        <v>1.438735087712606</v>
       </c>
       <c r="C8">
-        <v>0.09058797798411737</v>
+        <v>0.01249351092357862</v>
       </c>
       <c r="D8">
-        <v>0.2433849970499674</v>
+        <v>0.1918479601542155</v>
       </c>
       <c r="E8">
-        <v>0.02404784921160638</v>
+        <v>0.0009651264248244035</v>
       </c>
       <c r="F8" t="s">
         <v>16</v>
       </c>
       <c r="G8">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H8">
         <v>20</v>
@@ -936,19 +936,19 @@
         <v>26</v>
       </c>
       <c r="L8">
-        <v>0.9779411554336548</v>
+        <v>0.9632353186607361</v>
       </c>
       <c r="M8">
-        <v>0.9485294222831726</v>
+        <v>0.9632353186607361</v>
       </c>
       <c r="N8">
-        <v>0.9485294222831726</v>
+        <v>0.9411764740943909</v>
       </c>
       <c r="O8">
-        <v>0.9583333333333334</v>
+        <v>0.9558823704719543</v>
       </c>
       <c r="P8">
-        <v>0.01386482397143675</v>
+        <v>0.01039863905200182</v>
       </c>
       <c r="Q8">
         <v>7</v>
@@ -956,19 +956,19 @@
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="1">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9">
-        <v>1.307325045267741</v>
+        <v>1.338441769282023</v>
       </c>
       <c r="C9">
-        <v>0.008469805192483257</v>
+        <v>0.03254587046710085</v>
       </c>
       <c r="D9">
-        <v>0.2114369074503581</v>
+        <v>0.1905173460642497</v>
       </c>
       <c r="E9">
-        <v>0.008500484220290202</v>
+        <v>0.01326512495981162</v>
       </c>
       <c r="F9" t="s">
         <v>16</v>
@@ -980,7 +980,7 @@
         <v>23</v>
       </c>
       <c r="I9">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="J9" t="s">
         <v>18</v>
@@ -989,45 +989,45 @@
         <v>27</v>
       </c>
       <c r="L9">
-        <v>0.9779411554336548</v>
+        <v>0.9558823704719543</v>
       </c>
       <c r="M9">
-        <v>0.970588207244873</v>
+        <v>0.9632353186607361</v>
       </c>
       <c r="N9">
-        <v>0.9264705777168274</v>
+        <v>0.9485294222831726</v>
       </c>
       <c r="O9">
-        <v>0.9583333134651184</v>
+        <v>0.9558823704719543</v>
       </c>
       <c r="P9">
-        <v>0.02272945092152168</v>
+        <v>0.006003657055879005</v>
       </c>
       <c r="Q9">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:17">
       <c r="A10" s="1">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B10">
-        <v>1.617863416671753</v>
+        <v>1.483864068984985</v>
       </c>
       <c r="C10">
-        <v>0.1377167475790938</v>
+        <v>0.004758269612318707</v>
       </c>
       <c r="D10">
-        <v>0.2112774054209391</v>
+        <v>0.1921413739522298</v>
       </c>
       <c r="E10">
-        <v>0.004362390291052484</v>
+        <v>0.006184805196192857</v>
       </c>
       <c r="F10" t="s">
         <v>16</v>
       </c>
       <c r="G10">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H10">
         <v>23</v>
@@ -1042,19 +1042,19 @@
         <v>28</v>
       </c>
       <c r="L10">
-        <v>0.9558823704719543</v>
+        <v>0.9485294222831726</v>
       </c>
       <c r="M10">
-        <v>0.9558823704719543</v>
+        <v>0.970588207244873</v>
       </c>
       <c r="N10">
-        <v>0.9558823704719543</v>
+        <v>0.9485294222831726</v>
       </c>
       <c r="O10">
-        <v>0.9558823704719543</v>
+        <v>0.9558823506037394</v>
       </c>
       <c r="P10">
-        <v>0</v>
+        <v>0.01039861095410281</v>
       </c>
       <c r="Q10">
         <v>9</v>
@@ -1065,16 +1065,16 @@
         <v>7</v>
       </c>
       <c r="B11">
-        <v>1.204922596613566</v>
+        <v>1.082585493723552</v>
       </c>
       <c r="C11">
-        <v>0.07288831937205656</v>
+        <v>0.07859163232866567</v>
       </c>
       <c r="D11">
-        <v>0.2147659460703532</v>
+        <v>0.1974958578745524</v>
       </c>
       <c r="E11">
-        <v>0.005176424749405606</v>
+        <v>0.01269676994263839</v>
       </c>
       <c r="F11" t="s">
         <v>17</v>
@@ -1118,16 +1118,16 @@
         <v>1</v>
       </c>
       <c r="B12">
-        <v>1.319321791330973</v>
+        <v>1.227774222691854</v>
       </c>
       <c r="C12">
-        <v>0.0563045162104451</v>
+        <v>0.07287272818108996</v>
       </c>
       <c r="D12">
-        <v>0.2037890752156576</v>
+        <v>0.234753688176473</v>
       </c>
       <c r="E12">
-        <v>0.004701003291137693</v>
+        <v>0.06476628965756899</v>
       </c>
       <c r="F12" t="s">
         <v>17</v>
@@ -1171,16 +1171,16 @@
         <v>9</v>
       </c>
       <c r="B13">
-        <v>1.679850498835246</v>
+        <v>1.426222006479899</v>
       </c>
       <c r="C13">
-        <v>0.1725539412384311</v>
+        <v>0.02136155482336817</v>
       </c>
       <c r="D13">
-        <v>0.221262534459432</v>
+        <v>0.2549788951873779</v>
       </c>
       <c r="E13">
-        <v>0.01119606027167893</v>
+        <v>0.05916210091677459</v>
       </c>
       <c r="F13" t="s">
         <v>17</v>
@@ -1224,16 +1224,16 @@
         <v>11</v>
       </c>
       <c r="B14">
-        <v>1.350428342819214</v>
+        <v>1.331095774968465</v>
       </c>
       <c r="C14">
-        <v>0.1048472790502766</v>
+        <v>0.1527939722120929</v>
       </c>
       <c r="D14">
-        <v>0.2092833518981934</v>
+        <v>0.1958961486816406</v>
       </c>
       <c r="E14">
-        <v>0.004733681549182516</v>
+        <v>0.01015339952933555</v>
       </c>
       <c r="F14" t="s">
         <v>17</v>
@@ -1277,16 +1277,16 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>1.519797960917155</v>
+        <v>1.484998464584351</v>
       </c>
       <c r="C15">
-        <v>0.02251204204103448</v>
+        <v>0.146555641007668</v>
       </c>
       <c r="D15">
-        <v>0.2902418772379557</v>
+        <v>0.2089932759602865</v>
       </c>
       <c r="E15">
-        <v>0.07687311607115517</v>
+        <v>0.02060753130309324</v>
       </c>
       <c r="F15" t="s">
         <v>17</v>
@@ -1330,16 +1330,16 @@
         <v>3</v>
       </c>
       <c r="B16">
-        <v>1.150528192520142</v>
+        <v>1.15697455406189</v>
       </c>
       <c r="C16">
-        <v>0.01738449039092538</v>
+        <v>0.06185273010732815</v>
       </c>
       <c r="D16">
-        <v>0.2133869330088297</v>
+        <v>0.2156105041503906</v>
       </c>
       <c r="E16">
-        <v>0.008710268133208403</v>
+        <v>0.02402566689600774</v>
       </c>
       <c r="F16" t="s">
         <v>17</v>
@@ -1383,16 +1383,16 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>1.294785499572754</v>
+        <v>1.065202951431274</v>
       </c>
       <c r="C17">
-        <v>0.09894901058466678</v>
+        <v>0.02182598424148166</v>
       </c>
       <c r="D17">
-        <v>0.2167620658874512</v>
+        <v>0.1873187224070231</v>
       </c>
       <c r="E17">
-        <v>0.00283343071924997</v>
+        <v>0.004438567904341753</v>
       </c>
       <c r="F17" t="s">
         <v>17</v>
@@ -1436,16 +1436,16 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>1.602001428604126</v>
+        <v>1.451653877894084</v>
       </c>
       <c r="C18">
-        <v>0.03738051936090277</v>
+        <v>0.1094704084477465</v>
       </c>
       <c r="D18">
-        <v>0.2207480271657308</v>
+        <v>0.1933934688568115</v>
       </c>
       <c r="E18">
-        <v>0.0009448633136702844</v>
+        <v>0.002571413181164279</v>
       </c>
       <c r="F18" t="s">
         <v>16</v>
@@ -1489,16 +1489,16 @@
         <v>14</v>
       </c>
       <c r="B19">
-        <v>1.353089173634847</v>
+        <v>1.166177670160929</v>
       </c>
       <c r="C19">
-        <v>0.0464153557953832</v>
+        <v>0.1020510131576603</v>
       </c>
       <c r="D19">
-        <v>0.2280590534210205</v>
+        <v>0.1935568650563558</v>
       </c>
       <c r="E19">
-        <v>0.01647918336838871</v>
+        <v>0.002785906398081314</v>
       </c>
       <c r="F19" t="s">
         <v>17</v>
@@ -1542,16 +1542,16 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>1.391481637954712</v>
+        <v>1.298392136891683</v>
       </c>
       <c r="C20">
-        <v>0.01707199632492417</v>
+        <v>0.08894257412901597</v>
       </c>
       <c r="D20">
-        <v>0.2168051401774088</v>
+        <v>0.1936707496643066</v>
       </c>
       <c r="E20">
-        <v>0.001273270760300083</v>
+        <v>0.001413641800720539</v>
       </c>
       <c r="F20" t="s">
         <v>16</v>
@@ -1595,16 +1595,16 @@
         <v>12</v>
       </c>
       <c r="B21">
-        <v>1.56726598739624</v>
+        <v>1.34957234064738</v>
       </c>
       <c r="C21">
-        <v>0.05201058093838761</v>
+        <v>0.0538486776691988</v>
       </c>
       <c r="D21">
-        <v>0.2432063420613607</v>
+        <v>0.208854595820109</v>
       </c>
       <c r="E21">
-        <v>0.01428102142048551</v>
+        <v>0.01624616751259002</v>
       </c>
       <c r="F21" t="s">
         <v>17</v>
@@ -1648,16 +1648,16 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>1.592679023742676</v>
+        <v>1.442020177841187</v>
       </c>
       <c r="C22">
-        <v>0.08226030950143461</v>
+        <v>0.06958565720352516</v>
       </c>
       <c r="D22">
-        <v>0.3292238712310791</v>
+        <v>0.2082217534383138</v>
       </c>
       <c r="E22">
-        <v>0.1430204431127529</v>
+        <v>0.009714231276459326</v>
       </c>
       <c r="F22" t="s">
         <v>16</v>
@@ -1701,16 +1701,16 @@
         <v>10</v>
       </c>
       <c r="B23">
-        <v>1.361447095870972</v>
+        <v>1.204549392064412</v>
       </c>
       <c r="C23">
-        <v>0.007340461664833408</v>
+        <v>0.04604926540433585</v>
       </c>
       <c r="D23">
-        <v>0.2260482311248779</v>
+        <v>0.2179365158081055</v>
       </c>
       <c r="E23">
-        <v>0.006384490221784405</v>
+        <v>0.03037520476804687</v>
       </c>
       <c r="F23" t="s">
         <v>17</v>
@@ -1754,16 +1754,16 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>1.527614911397298</v>
+        <v>1.253485123316447</v>
       </c>
       <c r="C24">
-        <v>0.1065796594254622</v>
+        <v>0.05931350354222981</v>
       </c>
       <c r="D24">
-        <v>0.2323992252349854</v>
+        <v>0.2186075846354167</v>
       </c>
       <c r="E24">
-        <v>0.009155894051898336</v>
+        <v>0.0106986669830561</v>
       </c>
       <c r="F24" t="s">
         <v>16</v>
@@ -1807,16 +1807,16 @@
         <v>8</v>
       </c>
       <c r="B25">
-        <v>1.655205249786377</v>
+        <v>1.440659205118815</v>
       </c>
       <c r="C25">
-        <v>0.05277362404100611</v>
+        <v>0.07668703447023351</v>
       </c>
       <c r="D25">
-        <v>0.2220989068349203</v>
+        <v>0.2020050684611003</v>
       </c>
       <c r="E25">
-        <v>0.002459759002398355</v>
+        <v>0.01781002324768623</v>
       </c>
       <c r="F25" t="s">
         <v>17</v>
@@ -1860,16 +1860,16 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>1.933202505111694</v>
+        <v>1.629206260045369</v>
       </c>
       <c r="C26">
-        <v>0.027161124757386</v>
+        <v>0.003180396616607363</v>
       </c>
       <c r="D26">
-        <v>0.2376200358072917</v>
+        <v>0.2073059876759847</v>
       </c>
       <c r="E26">
-        <v>0.007203249351154245</v>
+        <v>0.007297415461090131</v>
       </c>
       <c r="F26" t="s">
         <v>16</v>
@@ -1913,16 +1913,16 @@
         <v>6</v>
       </c>
       <c r="B27">
-        <v>1.173621495564779</v>
+        <v>1.063268740971883</v>
       </c>
       <c r="C27">
-        <v>0.03747053906719948</v>
+        <v>0.07526196106719171</v>
       </c>
       <c r="D27">
-        <v>0.2221748828887939</v>
+        <v>0.1971870263417562</v>
       </c>
       <c r="E27">
-        <v>0.01048028375366202</v>
+        <v>0.01074059128559968</v>
       </c>
       <c r="F27" t="s">
         <v>17</v>
@@ -1966,16 +1966,16 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>1.701268752415975</v>
+        <v>1.38709290822347</v>
       </c>
       <c r="C28">
-        <v>0.06787326729822564</v>
+        <v>0.1210138911923623</v>
       </c>
       <c r="D28">
-        <v>0.2896305720011393</v>
+        <v>0.1933290163675944</v>
       </c>
       <c r="E28">
-        <v>0.07827780885215124</v>
+        <v>0.004117891186393967</v>
       </c>
       <c r="F28" t="s">
         <v>16</v>
@@ -2019,16 +2019,16 @@
         <v>4</v>
       </c>
       <c r="B29">
-        <v>1.366540908813477</v>
+        <v>1.239871025085449</v>
       </c>
       <c r="C29">
-        <v>0.08031899404674286</v>
+        <v>0.08392263267162249</v>
       </c>
       <c r="D29">
-        <v>0.2239500681559245</v>
+        <v>0.2076450983683268</v>
       </c>
       <c r="E29">
-        <v>0.01178110563706281</v>
+        <v>0.02629665789514475</v>
       </c>
       <c r="F29" t="s">
         <v>17</v>
@@ -2072,16 +2072,16 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>2.025091648101807</v>
+        <v>1.59277598063151</v>
       </c>
       <c r="C30">
-        <v>0.1420418372386166</v>
+        <v>0.1511821859890146</v>
       </c>
       <c r="D30">
-        <v>0.2382424672444662</v>
+        <v>0.1992182731628418</v>
       </c>
       <c r="E30">
-        <v>0.0121484160501257</v>
+        <v>0.004254577430877061</v>
       </c>
       <c r="F30" t="s">
         <v>16</v>
@@ -2125,16 +2125,16 @@
         <v>2</v>
       </c>
       <c r="B31">
-        <v>1.168798764546712</v>
+        <v>1.148667732874552</v>
       </c>
       <c r="C31">
-        <v>0.003927679090601844</v>
+        <v>0.0530295331988549</v>
       </c>
       <c r="D31">
-        <v>0.2587048212687175</v>
+        <v>0.2563321590423584</v>
       </c>
       <c r="E31">
-        <v>0.05277559643023595</v>
+        <v>0.0558452249877425</v>
       </c>
       <c r="F31" t="s">
         <v>17</v>
@@ -2178,16 +2178,16 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>1.572733084360759</v>
+        <v>1.224151293436686</v>
       </c>
       <c r="C32">
-        <v>0.03085221520852063</v>
+        <v>0.005879691318509608</v>
       </c>
       <c r="D32">
-        <v>0.2307629585266113</v>
+        <v>0.1971186796824137</v>
       </c>
       <c r="E32">
-        <v>0.01532511056346158</v>
+        <v>0.004934085212580121</v>
       </c>
       <c r="F32" t="s">
         <v>16</v>
@@ -2231,16 +2231,16 @@
         <v>0</v>
       </c>
       <c r="B33">
-        <v>1.451612949371338</v>
+        <v>1.403863747914632</v>
       </c>
       <c r="C33">
-        <v>0.06155652289499486</v>
+        <v>0.174752685186779</v>
       </c>
       <c r="D33">
-        <v>0.2275511423746745</v>
+        <v>0.1991113026936849</v>
       </c>
       <c r="E33">
-        <v>0.01126548431741047</v>
+        <v>0.02133169370007735</v>
       </c>
       <c r="F33" t="s">
         <v>17</v>

</xml_diff>